<commit_message>
Improved contract note parser with charge proration
- Changed section priority: prefer Equity Segment over Annexure B
  (Equity Segment is single-page, more reliable)
- Added Obligation Details parsing for STT, GST, exchange charges,
  SEBI fees, and stamp duty
- Implemented charge proration across transactions proportionally
  by trade value
- Enhanced security name cleaning (remove parenthesized qualifiers,
  handle multi-line cells)
- Updated effective price calculation to include all prorated charges

Data updates:
- Market ticker refresh (Gold: ₹156,200 +2.2%, Silver: ₹244,999 +0.26%,
  Crude Oil: ₹5,724 +0.67%)
- Stock price updates for portfolio holdings
- Added Triveni Turbine Limited to portfolio

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/dumps/Stocks/Adani Green Energy Limited.xlsx
+++ b/dumps/Stocks/Adani Green Energy Limited.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB7"/>
+  <dimension ref="A1:AB8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -574,11 +574,11 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46063</v>
+        <v>46066</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BSE</t>
+          <t>NSE</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -590,18 +590,21 @@
         <v>5</v>
       </c>
       <c r="E5" t="n">
-        <v>978.4</v>
+        <v>952.35</v>
       </c>
       <c r="F5" t="n">
-        <v>4916.45</v>
+        <v>4795.29</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>CN#252611730667</t>
-        </is>
+          <t>CN#252611910666</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>4.81</v>
       </c>
       <c r="I5" t="n">
-        <v>24.45</v>
+        <v>28.732</v>
       </c>
       <c r="J5">
         <f>Index!$C$2</f>
@@ -610,11 +613,11 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>46059</v>
+        <v>46063</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>NSE</t>
+          <t>BSE</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -626,18 +629,18 @@
         <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>961</v>
+        <v>978.4</v>
       </c>
       <c r="F6" t="n">
-        <v>4829.05</v>
+        <v>4916.45</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>CN#252611604850</t>
+          <t>CN#252611730667</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>24.05</v>
+        <v>24.45</v>
       </c>
       <c r="J6">
         <f>Index!$C$2</f>
@@ -646,7 +649,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -662,20 +665,56 @@
         <v>5</v>
       </c>
       <c r="E7" t="n">
+        <v>961</v>
+      </c>
+      <c r="F7" t="n">
+        <v>4829.05</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>CN#252611604850</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>24.05</v>
+      </c>
+      <c r="J7">
+        <f>Index!$C$2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>46057</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>5</v>
+      </c>
+      <c r="E8" t="n">
         <v>957.7</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F8" t="n">
         <v>4812.45</v>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>CN#252611485581</t>
         </is>
       </c>
-      <c r="I7" t="n">
+      <c r="I8" t="n">
         <v>23.95</v>
       </c>
-      <c r="J7">
+      <c r="J8">
         <f>Index!$C$2</f>
         <v/>
       </c>

</xml_diff>